<commit_message>
update eval test + pdf
</commit_message>
<xml_diff>
--- a/Template/findings/table4.xlsx
+++ b/Template/findings/table4.xlsx
@@ -414,27 +414,27 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>1.21</t>
+          <t>1.21***</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>1.25</t>
+          <t>1.25**</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>1.21</t>
+          <t>1.21**</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>1.21</t>
+          <t>1.21*</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>1.21</t>
+          <t>1.21**</t>
         </is>
       </c>
     </row>
@@ -549,27 +549,27 @@
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
+          <t>1.46***</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
           <t>1.46**</t>
         </is>
       </c>
-      <c r="B8" t="inlineStr">
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>1.5***</t>
+        </is>
+      </c>
+      <c r="D8" t="inlineStr">
         <is>
           <t>1.46**</t>
         </is>
       </c>
-      <c r="C8" t="inlineStr">
-        <is>
-          <t>1.5**</t>
-        </is>
-      </c>
-      <c r="D8" t="inlineStr">
-        <is>
-          <t>1.46**</t>
-        </is>
-      </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>1.39*</t>
+          <t>1.39***</t>
         </is>
       </c>
     </row>
@@ -819,27 +819,27 @@
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>1.54***</t>
+          <t>1.54</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>1.57***</t>
+          <t>1.57</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>1.57***</t>
+          <t>1.57*</t>
         </is>
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>1.5**</t>
+          <t>1.5</t>
         </is>
       </c>
       <c r="E18" t="inlineStr">
         <is>
-          <t>1.61***</t>
+          <t>1.61</t>
         </is>
       </c>
     </row>
@@ -900,12 +900,12 @@
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>0.01***</t>
+          <t>0.01</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>18.99***</t>
+          <t>18.99**</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
@@ -915,7 +915,7 @@
       </c>
       <c r="D21" t="inlineStr">
         <is>
-          <t>17.38***</t>
+          <t>17.38**</t>
         </is>
       </c>
       <c r="E21" t="inlineStr">

</xml_diff>